<commit_message>
Before making changes to ALICE plots
</commit_message>
<xml_diff>
--- a/data-raw/2020-obtn-by-county.xlsx
+++ b/data-raw/2020-obtn-by-county.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caplans\Dropbox\ ObtN 2019-2020\2020 ObtN\2020 ObtN Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidkeyes/Documents/Work/TFFF/OBTN/obtn/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF93A5A-E2EB-2C4E-AB1D-09F59008AC13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35160" yWindow="1185" windowWidth="26805" windowHeight="16035"/>
+    <workbookView xWindow="35160" yWindow="1180" windowWidth="26800" windowHeight="16040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Population" sheetId="6" r:id="rId1"/>
@@ -672,9 +673,6 @@
     <t>Coos Bay</t>
   </si>
   <si>
-    <t>Prinville</t>
-  </si>
-  <si>
     <t>Brookings</t>
   </si>
   <si>
@@ -826,12 +824,15 @@
   </si>
   <si>
     <t>Computer and Electronic Product Manufacturing</t>
+  </si>
+  <si>
+    <t>Prineville</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -1222,14 +1223,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
@@ -1557,16 +1558,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="102">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="112">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2733,16 +2734,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AK40"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:37" s="5" customFormat="1" ht="25.5">
+    <row r="1" spans="1:37" s="5" customFormat="1" ht="28">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7268,16 +7269,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="14">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7296,13 +7297,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" t="s">
         <v>245</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>246</v>
-      </c>
-      <c r="D2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15">
@@ -7310,13 +7311,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" t="s">
         <v>245</v>
       </c>
-      <c r="C3" t="s">
-        <v>246</v>
-      </c>
       <c r="D3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15">
@@ -7324,13 +7325,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15">
@@ -7338,13 +7339,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15">
@@ -7352,13 +7353,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15">
@@ -7366,13 +7367,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15">
@@ -7380,13 +7381,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15">
@@ -7394,13 +7395,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15">
@@ -7408,13 +7409,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" t="s">
         <v>246</v>
       </c>
-      <c r="C10" t="s">
-        <v>247</v>
-      </c>
       <c r="D10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15">
@@ -7422,13 +7423,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15">
@@ -7436,13 +7437,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>251</v>
+      </c>
+      <c r="C12" t="s">
         <v>252</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>253</v>
-      </c>
-      <c r="D12" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15">
@@ -7450,13 +7451,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15">
@@ -7464,13 +7465,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" t="s">
         <v>245</v>
-      </c>
-      <c r="C14" t="s">
-        <v>236</v>
-      </c>
-      <c r="D14" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15">
@@ -7478,13 +7479,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15">
@@ -7492,13 +7493,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>245</v>
+      </c>
+      <c r="C16" t="s">
         <v>246</v>
       </c>
-      <c r="C16" t="s">
-        <v>247</v>
-      </c>
       <c r="D16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15">
@@ -7506,13 +7507,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>244</v>
+      </c>
+      <c r="C17" t="s">
         <v>245</v>
       </c>
-      <c r="C17" t="s">
-        <v>246</v>
-      </c>
       <c r="D17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15">
@@ -7520,13 +7521,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>245</v>
+      </c>
+      <c r="C18" t="s">
+        <v>244</v>
+      </c>
+      <c r="D18" t="s">
         <v>246</v>
-      </c>
-      <c r="C18" t="s">
-        <v>245</v>
-      </c>
-      <c r="D18" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15">
@@ -7534,13 +7535,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" t="s">
         <v>245</v>
       </c>
-      <c r="C19" t="s">
-        <v>246</v>
-      </c>
       <c r="D19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15">
@@ -7548,13 +7549,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15">
@@ -7562,13 +7563,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>244</v>
+      </c>
+      <c r="C21" t="s">
         <v>245</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>246</v>
-      </c>
-      <c r="D21" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15">
@@ -7576,13 +7577,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15">
@@ -7590,13 +7591,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>244</v>
+      </c>
+      <c r="C23" t="s">
         <v>245</v>
       </c>
-      <c r="C23" t="s">
-        <v>246</v>
-      </c>
       <c r="D23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15">
@@ -7604,13 +7605,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>244</v>
+      </c>
+      <c r="C24" t="s">
         <v>245</v>
       </c>
-      <c r="C24" t="s">
-        <v>246</v>
-      </c>
       <c r="D24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15">
@@ -7618,13 +7619,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>245</v>
+      </c>
+      <c r="C25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D25" t="s">
         <v>246</v>
-      </c>
-      <c r="C25" t="s">
-        <v>245</v>
-      </c>
-      <c r="D25" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15">
@@ -7632,13 +7633,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>258</v>
+      </c>
+      <c r="C26" t="s">
+        <v>255</v>
+      </c>
+      <c r="D26" t="s">
         <v>259</v>
-      </c>
-      <c r="C26" t="s">
-        <v>256</v>
-      </c>
-      <c r="D26" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15">
@@ -7646,13 +7647,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>244</v>
+      </c>
+      <c r="C27" t="s">
         <v>245</v>
       </c>
-      <c r="C27" t="s">
-        <v>246</v>
-      </c>
       <c r="D27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15">
@@ -7660,13 +7661,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>244</v>
+      </c>
+      <c r="C28" t="s">
         <v>245</v>
       </c>
-      <c r="C28" t="s">
-        <v>246</v>
-      </c>
       <c r="D28" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15">
@@ -7674,13 +7675,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15">
@@ -7688,13 +7689,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15">
@@ -7702,13 +7703,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15">
@@ -7716,13 +7717,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>244</v>
+      </c>
+      <c r="C32" t="s">
         <v>245</v>
       </c>
-      <c r="C32" t="s">
-        <v>246</v>
-      </c>
       <c r="D32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15">
@@ -7730,13 +7731,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15">
@@ -7744,13 +7745,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15">
@@ -7758,13 +7759,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C35" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D35" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15">
@@ -7772,13 +7773,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C36" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D36" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15">
@@ -7786,13 +7787,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>244</v>
+      </c>
+      <c r="C37" t="s">
         <v>245</v>
       </c>
-      <c r="C37" t="s">
-        <v>246</v>
-      </c>
       <c r="D37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15">
@@ -7810,13 +7811,13 @@
         <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C40" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -7825,16 +7826,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
@@ -7842,13 +7843,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1">
@@ -8369,16 +8370,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
@@ -8386,13 +8387,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1">
@@ -8928,16 +8929,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -9260,16 +9261,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -9598,16 +9599,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -9936,16 +9937,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -10274,17 +10275,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
@@ -10369,7 +10370,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>211</v>
+        <v>262</v>
       </c>
       <c r="C8">
         <v>9748</v>
@@ -10380,7 +10381,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C9">
         <v>6413</v>
@@ -10391,7 +10392,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C10">
         <v>90500</v>
@@ -10402,7 +10403,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C11">
         <v>22988</v>
@@ -10413,7 +10414,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C12">
         <v>655</v>
@@ -10424,7 +10425,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C13">
         <v>2251</v>
@@ -10435,7 +10436,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C14">
         <v>2756</v>
@@ -10457,7 +10458,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C16">
         <v>80051</v>
@@ -10468,7 +10469,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C17">
         <v>6674</v>
@@ -10479,7 +10480,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C18">
         <v>37201</v>
@@ -10490,7 +10491,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C19">
         <v>21138</v>
@@ -10501,7 +10502,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C20">
         <v>2765</v>
@@ -10512,7 +10513,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C21">
         <v>165997</v>
@@ -10523,7 +10524,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C22">
         <v>10381</v>
@@ -10534,7 +10535,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C23">
         <v>52736</v>
@@ -10545,7 +10546,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C24">
         <v>10997</v>
@@ -10556,7 +10557,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C25">
         <v>166756</v>
@@ -10567,7 +10568,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C26">
         <v>3340</v>
@@ -10589,7 +10590,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C28">
         <v>166756</v>
@@ -10622,7 +10623,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C31">
         <v>17346</v>
@@ -10633,7 +10634,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C32">
         <v>13103</v>
@@ -10644,7 +10645,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C33">
         <v>1990</v>
@@ -10655,7 +10656,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C34">
         <v>15320</v>
@@ -10677,7 +10678,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C36">
         <v>503</v>
@@ -10688,7 +10689,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C37">
         <v>33662</v>
@@ -10709,16 +10710,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
@@ -10743,7 +10744,7 @@
         <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D2" t="s">
         <v>108</v>
@@ -11254,14 +11255,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
@@ -11676,7 +11677,7 @@
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="8" t="s">
@@ -11710,7 +11711,7 @@
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="8" t="s">
@@ -11728,7 +11729,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="8" t="s">
@@ -11760,7 +11761,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8" t="s">
@@ -11840,7 +11841,7 @@
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
@@ -11872,7 +11873,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8" t="s">
@@ -11887,16 +11888,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>